<commit_message>
fixed the issue with the heat pump
</commit_message>
<xml_diff>
--- a/export/change reports/change_report 2023-10-12.xlsx
+++ b/export/change reports/change_report 2023-10-12.xlsx
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="C2" s="1" t="n">
-        <v>45211.59965800553</v>
+        <v>45211.64983435021</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3545,6 +3545,2931 @@
         </is>
       </c>
     </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:25,778</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, LFP</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:25,779</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>market group for heat, district or industrial, natural gas</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>RER</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:25,779</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NMC811</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:25,779</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NMC811</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:25,780</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NCA</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:25,781</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>market group for heat, district or industrial, natural gas</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:25,781</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>market for heat pump, heat and power co-generation unit, 160kW electrical</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:25,781</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NCA</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:25,782</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, LFP</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:25,782</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>battery cell production, NMC-622</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:25,782</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>battery cell production, PLIB</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:26,342</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>market for battery cell production</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2023-10-12 14:54:26,363</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>market for heat</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:51,777</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, LFP</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:51,778</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>market group for heat, district or industrial, natural gas</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>RER</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:51,778</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NMC811</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:51,778</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NMC811</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:51,779</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NCA</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:51,779</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>market group for heat, district or industrial, natural gas</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:51,779</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>market for heat pump, heat and power co-generation unit, 160kW electrical</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:51,779</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NCA</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:51,780</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, LFP</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:51,780</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>battery cell production, NMC-622</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:51,780</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>battery cell production, PLIB</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:52,240</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>market for battery cell production</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:52,260</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>market for heat</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:53,747</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, LFP</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:53,748</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G96" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>market group for heat, district or industrial, natural gas</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>RER</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:53,748</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G97" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NMC811</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:53,748</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G98" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NMC811</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:53,749</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G99" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NCA</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:53,749</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G100" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>market group for heat, district or industrial, natural gas</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:53,749</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G101" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>market for heat pump, heat and power co-generation unit, 160kW electrical</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:53,749</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G102" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NCA</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:53,750</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G103" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, LFP</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:53,750</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G104" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>battery cell production, NMC-622</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:53,750</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G105" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>battery cell production, PLIB</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:54,128</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G106" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>market for battery cell production</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:54,141</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>SSP2-Base</t>
+        </is>
+      </c>
+      <c r="G107" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>market for heat</t>
+        </is>
+      </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:55,697</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G108" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, LFP</t>
+        </is>
+      </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:55,698</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G109" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>market group for heat, district or industrial, natural gas</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>RER</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:55,698</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G110" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NMC811</t>
+        </is>
+      </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:55,698</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G111" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NMC811</t>
+        </is>
+      </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:55,698</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G112" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NCA</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:55,699</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G113" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>market group for heat, district or industrial, natural gas</t>
+        </is>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:55,699</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G114" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>market for heat pump, heat and power co-generation unit, 160kW electrical</t>
+        </is>
+      </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:55,699</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G115" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NCA</t>
+        </is>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:55,699</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G116" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, LFP</t>
+        </is>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:55,699</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G117" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>battery cell production, NMC-622</t>
+        </is>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:55,699</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G118" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>battery cell production, PLIB</t>
+        </is>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:56,463</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G119" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>market for battery cell production</t>
+        </is>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:56,477</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G120" t="n">
+        <v>2021</v>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>market for heat</t>
+        </is>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:57,702</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G121" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, LFP</t>
+        </is>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:57,702</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G122" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>market group for heat, district or industrial, natural gas</t>
+        </is>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>RER</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:57,702</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G123" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NMC811</t>
+        </is>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:57,703</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G124" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NMC811</t>
+        </is>
+      </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:57,703</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G125" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NCA</t>
+        </is>
+      </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:57,703</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G126" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>market group for heat, district or industrial, natural gas</t>
+        </is>
+      </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:57,704</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G127" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>market for heat pump, heat and power co-generation unit, 160kW electrical</t>
+        </is>
+      </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:57,704</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G128" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, NCA</t>
+        </is>
+      </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:57,704</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G129" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>battery cell production, Li-ion, LFP</t>
+        </is>
+      </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>RoW</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:57,704</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G130" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>battery cell production, NMC-622</t>
+        </is>
+      </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:57,704</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>updated</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G131" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>battery cell production, PLIB</t>
+        </is>
+      </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:58,081</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G132" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>market for battery cell production</t>
+        </is>
+      </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2023-10-12 15:32:58,099</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>external</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>INFO</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>created</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>SSP2-RCP26</t>
+        </is>
+      </c>
+      <c r="G133" t="n">
+        <v>2040</v>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>market for heat</t>
+        </is>
+      </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>GLO</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>